<commit_message>
Fixing and Scripting  SCD0260 - SCD0270
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_Digisales/SCD0260 - Searching profiling nasabah & memiliki sales kelolaan.xlsx
+++ b/Lib_Repo_Excel/FileExcel_Digisales/SCD0260 - Searching profiling nasabah & memiliki sales kelolaan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C28CC7A-0614-4CBB-9F58-14F44D47E472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48491805-4D07-4D12-BDE0-69B8F9A8BCF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SCD0260" sheetId="2" r:id="rId1"/>
@@ -149,7 +149,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,6 +181,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -202,7 +209,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -221,9 +228,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -233,6 +237,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -541,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0EAF5E5-8229-45B3-AC11-8AED029F52F4}">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="I4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5:O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,7 +567,7 @@
     <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.140625" customWidth="1"/>
     <col min="16" max="16" width="25" customWidth="1"/>
@@ -623,7 +631,7 @@
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>20</v>
       </c>
       <c r="C2" s="8" t="s">
@@ -635,10 +643,10 @@
       <c r="E2" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="9">
-        <v>55210</v>
-      </c>
-      <c r="G2" s="10" t="s">
+      <c r="F2" s="12">
+        <v>35758</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>9</v>
       </c>
       <c r="H2" s="7" t="s">
@@ -648,16 +656,16 @@
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
-      <c r="M2" s="7">
-        <v>9315565540</v>
-      </c>
-      <c r="N2" s="11" t="s">
+      <c r="M2" s="12">
+        <v>9720826341</v>
+      </c>
+      <c r="N2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="13">
-        <v>9736118354</v>
-      </c>
-      <c r="P2" s="12" t="s">
+      <c r="O2" s="14">
+        <v>9669179367</v>
+      </c>
+      <c r="P2" s="11" t="s">
         <v>19</v>
       </c>
       <c r="Q2" s="7"/>
@@ -668,7 +676,7 @@
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>20</v>
       </c>
       <c r="C3" s="8" t="s">
@@ -681,9 +689,9 @@
         <v>22</v>
       </c>
       <c r="F3" s="13">
-        <v>32362</v>
-      </c>
-      <c r="G3" s="10" t="s">
+        <v>35795</v>
+      </c>
+      <c r="G3" s="9" t="s">
         <v>9</v>
       </c>
       <c r="H3" s="7" t="s">
@@ -700,7 +708,7 @@
       <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="12" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="8" t="s">
@@ -712,10 +720,10 @@
       <c r="E4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="13">
-        <v>19331</v>
-      </c>
-      <c r="G4" s="10" t="s">
+      <c r="F4" s="12">
+        <v>19256</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>9</v>
       </c>
       <c r="H4" s="7" t="s">
@@ -725,7 +733,7 @@
         <v>25</v>
       </c>
       <c r="J4" s="3"/>
-      <c r="O4" s="13"/>
+      <c r="O4" s="12"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="3"/>
       <c r="R4" s="2"/>
@@ -734,7 +742,7 @@
       <c r="A5" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="12" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="8" t="s">
@@ -746,10 +754,10 @@
       <c r="E5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="9">
-        <v>55210</v>
-      </c>
-      <c r="G5" s="10" t="s">
+      <c r="F5" s="12">
+        <v>35758</v>
+      </c>
+      <c r="G5" s="9" t="s">
         <v>9</v>
       </c>
       <c r="H5" s="7" t="s">
@@ -765,16 +773,16 @@
       <c r="L5" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="M5" s="7">
-        <v>9315565540</v>
-      </c>
-      <c r="N5" s="11" t="s">
+      <c r="M5" s="12">
+        <v>9720826341</v>
+      </c>
+      <c r="N5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="O5" s="13">
-        <v>9736118354</v>
-      </c>
-      <c r="P5" s="12"/>
+      <c r="O5" s="14">
+        <v>9669179367</v>
+      </c>
+      <c r="P5" s="11"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>

</xml_diff>